<commit_message>
atualizei trab no excel
</commit_message>
<xml_diff>
--- a/trabalho.xlsx
+++ b/trabalho.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Sujeito a</t>
   </si>
@@ -139,6 +139,21 @@
   </si>
   <si>
     <t>0,4y1 + 0,1y2 + 0,6y3 + 0,15y4 + 0,1y5 &gt;= 1</t>
+  </si>
+  <si>
+    <t>diesel</t>
+  </si>
+  <si>
+    <t>gasolina</t>
+  </si>
+  <si>
+    <t>lubrificante</t>
+  </si>
+  <si>
+    <t>combustível para jatos</t>
+  </si>
+  <si>
+    <t>óleo cru</t>
   </si>
 </sst>
 </file>
@@ -267,9 +282,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -301,6 +313,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,7 +616,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -616,84 +629,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="13"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
@@ -704,10 +729,10 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -723,139 +748,139 @@
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>54.999999999999993</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>30.000000000000007</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <f>(B15*B16)+(C15*C16)</f>
         <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="6">
+      <c r="A21" s="5">
         <v>1</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>-0.6</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>0.4</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <f>(B21*B$16)+(C21*C$16)</f>
         <v>-20.999999999999989</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>2</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>0.2</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>0.1</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <f>(B22*B$16)+(C22*C$16)</f>
         <v>14</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="6">
+      <c r="A23" s="5">
         <v>3</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>0.25</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>0.6</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <f>(B23*B$16)+(C23*C$16)</f>
         <v>31.75</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="6">
+      <c r="A24" s="5">
         <v>4</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>0.1</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>0.15</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <f>(B24*B$16)+(C24*C$16)</f>
         <v>10</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="6">
+      <c r="A25" s="5">
         <v>5</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>0.15</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>0.1</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <f>(B25*B$16)+(C25*C$16)</f>
         <v>11.25</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>8</v>
       </c>
     </row>

</xml_diff>